<commit_message>
typed lines, update MovementFactory, fix steps.xlsx
</commit_message>
<xml_diff>
--- a/public/steps.xlsx
+++ b/public/steps.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="97">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">правая</t>
   </si>
   <si>
-    <t xml:space="preserve">наружнее</t>
+    <t xml:space="preserve">наружное</t>
   </si>
   <si>
     <t xml:space="preserve">Кроссрол вперёд на правой</t>
@@ -94,34 +94,31 @@
     <t xml:space="preserve">Внутренний аксель на левой</t>
   </si>
   <si>
-    <t xml:space="preserve">внутренее</t>
-  </si>
-  <si>
     <t xml:space="preserve">Внутренний аксель на правой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль внутрь вправо на правой</t>
+    <t xml:space="preserve">Циркуль вперед внутрь на правой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль внутрь влево на правой</t>
+    <t xml:space="preserve">Циркуль назад внутрь на правой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль наружу влево на правой</t>
+    <t xml:space="preserve">Циркуль вперед наружу на правой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль наружу вправо на правой</t>
+    <t xml:space="preserve">Циркуль назад наружу на правой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль внутрь вправо на левой</t>
+    <t xml:space="preserve">Циркуль назад внутрь на левой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль внутрь влево на левой</t>
+    <t xml:space="preserve">Циркуль вперед внутрь на левой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль наружу влево на левой</t>
+    <t xml:space="preserve">Циркуль назад наружу на левой</t>
   </si>
   <si>
-    <t xml:space="preserve">Циркуль наружу вправо на левой</t>
+    <t xml:space="preserve">Циркуль вперед наружу на левой</t>
   </si>
   <si>
     <t xml:space="preserve">Козлик на правой</t>
@@ -152,9 +149,6 @@
   </si>
   <si>
     <t xml:space="preserve">Выпад назад внутрь на правой</t>
-  </si>
-  <si>
-    <t xml:space="preserve">правая.</t>
   </si>
   <si>
     <t xml:space="preserve">Выпад назад внутрь на левой</t>
@@ -767,9 +761,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>467640</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:colOff>466920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -782,8 +776,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16163280" y="2384640"/>
-          <a:ext cx="8497080" cy="7143120"/>
+          <a:off x="16668720" y="3089160"/>
+          <a:ext cx="8519400" cy="7142400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -805,13 +799,13 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G87" activeCellId="0" sqref="G87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
@@ -846,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -879,7 +873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -905,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
@@ -934,7 +928,7 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
         <v>18</v>
       </c>
@@ -963,7 +957,7 @@
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
         <v>19</v>
       </c>
@@ -992,7 +986,7 @@
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
         <v>20</v>
       </c>
@@ -1021,7 +1015,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="s">
         <v>21</v>
       </c>
@@ -1050,7 +1044,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1073,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
@@ -1089,8 +1083,8 @@
       <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>24</v>
+      <c r="D10" s="29" t="s">
+        <v>10</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>10</v>
@@ -1105,9 +1099,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>16</v>
@@ -1119,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F11" s="12" t="n">
         <v>0</v>
@@ -1131,9 +1125,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>16</v>
@@ -1147,8 +1141,8 @@
       <c r="E12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>11</v>
+      <c r="F12" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="G12" s="13" t="n">
         <v>-180</v>
@@ -1157,9 +1151,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>16</v>
@@ -1173,8 +1167,8 @@
       <c r="E13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>11</v>
+      <c r="F13" s="12" t="n">
+        <v>180</v>
       </c>
       <c r="G13" s="13" t="n">
         <v>180</v>
@@ -1183,9 +1177,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>16</v>
@@ -1209,9 +1203,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>16</v>
@@ -1235,9 +1229,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>15</v>
@@ -1261,9 +1255,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>15</v>
@@ -1287,9 +1281,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>15</v>
@@ -1313,9 +1307,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>15</v>
@@ -1339,9 +1333,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>15</v>
@@ -1350,10 +1344,10 @@
         <v>16</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="12" t="n">
         <v>0</v>
@@ -1365,9 +1359,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>16</v>
@@ -1376,10 +1370,10 @@
         <v>15</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="12" t="n">
         <v>0</v>
@@ -1391,9 +1385,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>16</v>
@@ -1417,9 +1411,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>15</v>
@@ -1443,9 +1437,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>16</v>
@@ -1469,9 +1463,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>15</v>
@@ -1495,9 +1489,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>16</v>
@@ -1521,9 +1515,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>15</v>
@@ -1547,15 +1541,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>10</v>
@@ -1573,9 +1567,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>15</v>
@@ -1599,9 +1593,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>16</v>
@@ -1610,10 +1604,10 @@
         <v>16</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" s="12" t="n">
         <v>0</v>
@@ -1625,9 +1619,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>15</v>
@@ -1636,10 +1630,10 @@
         <v>15</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="12" t="n">
         <v>0</v>
@@ -1651,9 +1645,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>16</v>
@@ -1662,10 +1656,10 @@
         <v>16</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="12" t="n">
         <v>180</v>
@@ -1677,9 +1671,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>15</v>
@@ -1688,10 +1682,10 @@
         <v>15</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="12" t="n">
         <v>180</v>
@@ -1703,9 +1697,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>16</v>
@@ -1732,9 +1726,9 @@
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>15</v>
@@ -1761,9 +1755,9 @@
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>16</v>
@@ -1790,9 +1784,9 @@
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>15</v>
@@ -1819,9 +1813,9 @@
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>9</v>
@@ -1845,9 +1839,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>9</v>
@@ -1871,9 +1865,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>9</v>
@@ -1897,9 +1891,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>9</v>
@@ -1923,9 +1917,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>9</v>
@@ -1949,9 +1943,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>9</v>
@@ -1975,9 +1969,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>9</v>
@@ -2001,9 +1995,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>9</v>
@@ -2027,9 +2021,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>15</v>
@@ -2038,10 +2032,10 @@
         <v>16</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F46" s="12" t="n">
         <v>0</v>
@@ -2053,9 +2047,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>16</v>
@@ -2064,10 +2058,10 @@
         <v>15</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F47" s="12" t="n">
         <v>0</v>
@@ -2079,9 +2073,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>16</v>
@@ -2090,10 +2084,10 @@
         <v>16</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" s="12" t="n">
         <v>0</v>
@@ -2105,9 +2099,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>15</v>
@@ -2116,10 +2110,10 @@
         <v>15</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F49" s="12" t="n">
         <v>0</v>
@@ -2131,9 +2125,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>16</v>
@@ -2142,10 +2136,10 @@
         <v>16</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F50" s="12" t="n">
         <v>180</v>
@@ -2157,9 +2151,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>15</v>
@@ -2168,10 +2162,10 @@
         <v>15</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F51" s="12" t="n">
         <v>180</v>
@@ -2183,9 +2177,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>16</v>
@@ -2209,9 +2203,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>16</v>
@@ -2235,9 +2229,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>16</v>
@@ -2261,9 +2255,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>16</v>
@@ -2287,9 +2281,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>15</v>
@@ -2313,9 +2307,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>15</v>
@@ -2339,9 +2333,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>15</v>
@@ -2365,9 +2359,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>15</v>
@@ -2391,9 +2385,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>16</v>
@@ -2417,9 +2411,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>16</v>
@@ -2443,9 +2437,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>16</v>
@@ -2469,9 +2463,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>16</v>
@@ -2495,9 +2489,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>15</v>
@@ -2521,9 +2515,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>15</v>
@@ -2547,9 +2541,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B66" s="10" t="s">
         <v>15</v>
@@ -2573,9 +2567,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>15</v>
@@ -2599,9 +2593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B68" s="10" t="s">
         <v>16</v>
@@ -2628,9 +2622,9 @@
       <c r="J68" s="15"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B69" s="10" t="s">
         <v>15</v>
@@ -2654,9 +2648,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>16</v>
@@ -2680,9 +2674,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B71" s="10" t="s">
         <v>15</v>
@@ -2706,9 +2700,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B72" s="10" t="s">
         <v>16</v>
@@ -2732,9 +2726,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B73" s="10" t="s">
         <v>15</v>
@@ -2758,9 +2752,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B74" s="10" t="s">
         <v>16</v>
@@ -2784,9 +2778,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B75" s="10" t="s">
         <v>15</v>
@@ -2810,9 +2804,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>16</v>
@@ -2836,9 +2830,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B77" s="10" t="s">
         <v>15</v>
@@ -2862,9 +2856,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B78" s="10" t="s">
         <v>16</v>
@@ -2888,9 +2882,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B79" s="10" t="s">
         <v>15</v>
@@ -2914,9 +2908,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B80" s="10" t="s">
         <v>16</v>
@@ -2940,9 +2934,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B81" s="10" t="s">
         <v>15</v>
@@ -2968,7 +2962,7 @@
     </row>
     <row r="82" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B82" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add columnName for distance
</commit_message>
<xml_diff>
--- a/public/steps.xlsx
+++ b/public/steps.xlsx
@@ -1370,11 +1370,11 @@
   <dimension ref="A1:P998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E146" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="L155" activeCellId="0" sqref="L155:L157"/>
+      <selection pane="bottomLeft" activeCell="A146" activeCellId="0" sqref="A146"/>
+      <selection pane="bottomRight" activeCell="H154" activeCellId="0" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>